<commit_message>
fix GameSetting sheet name
</commit_message>
<xml_diff>
--- a/excel/GameData.xlsx
+++ b/excel/GameData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geukg\OneDrive\문서\TSomSomm\lunaria-project\lunaria-data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560C7EC4-5B41-4689-B71C-8797A4103DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AE3383-FE84-4B50-A44E-0383B64B7697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1740" windowWidth="23715" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EnumData" sheetId="1" r:id="rId1"/>
+    <sheet name="GameSettingData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -459,7 +459,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>